<commit_message>
Restart the update in Fri, before taking in other teammates' work.
</commit_message>
<xml_diff>
--- a/Doc/Plan02/用例信息分工.xlsx
+++ b/Doc/Plan02/用例信息分工.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15945" windowHeight="12060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15948" windowHeight="12060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -619,16 +619,16 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.25" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -639,7 +639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -650,7 +650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
@@ -658,7 +658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
@@ -666,7 +666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -677,7 +677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
@@ -685,7 +685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
@@ -693,7 +693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -704,7 +704,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
@@ -712,7 +712,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
@@ -720,7 +720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
@@ -728,7 +728,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>17</v>
       </c>
@@ -736,7 +736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -744,7 +744,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -752,52 +752,52 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>31</v>
       </c>
@@ -805,7 +805,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>32</v>
       </c>

</xml_diff>